<commit_message>
Changes to event code adjustments, rank of ICA, epoch binning and visualization
</commit_message>
<xml_diff>
--- a/SupportingDocs/AR_Parameters_for_MW_Blinks.xlsx
+++ b/SupportingDocs/AR_Parameters_for_MW_Blinks.xlsx
@@ -13,7 +13,607 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="336">
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
   <si>
     <t>SUBID</t>
   </si>
@@ -441,7 +1041,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -466,11 +1066,36 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -489,6 +1114,31 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,41 +1151,41 @@
   <dimension ref="A1:G2"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.2578125" customWidth="true"/>
-    <col min="2" max="2" width="10.07421875" customWidth="true"/>
-    <col min="3" max="3" width="9.53125" customWidth="true"/>
-    <col min="4" max="4" width="21.2578125" customWidth="true"/>
-    <col min="5" max="5" width="21.62109375" customWidth="true"/>
-    <col min="6" max="6" width="11.8046875" customWidth="true"/>
-    <col min="7" max="7" width="12.2578125" customWidth="true"/>
+    <col min="1" max="1" width="6.42578125" customWidth="true"/>
+    <col min="2" max="2" width="10.7109375" customWidth="true"/>
+    <col min="3" max="3" width="10" customWidth="true"/>
+    <col min="4" max="4" width="22.42578125" customWidth="true"/>
+    <col min="5" max="5" width="22.7109375" customWidth="true"/>
+    <col min="6" max="6" width="12.5703125" customWidth="true"/>
+    <col min="7" max="7" width="13" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>128</v>
+        <v>328</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>130</v>
+        <v>330</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>131</v>
+        <v>331</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>132</v>
+        <v>332</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>133</v>
+        <v>333</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>134</v>
+        <v>334</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>135</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>129</v>
+        <v>329</v>
       </c>
       <c r="B2" s="0">
         <v>71</v>

</xml_diff>

<commit_message>
Corrected how event codes were shifted (errors in X1b)
</commit_message>
<xml_diff>
--- a/SupportingDocs/AR_Parameters_for_MW_Blinks.xlsx
+++ b/SupportingDocs/AR_Parameters_for_MW_Blinks.xlsx
@@ -13,7 +13,223 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="408">
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
   <si>
     <t>SUBID</t>
   </si>
@@ -1041,7 +1257,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1091,11 +1307,20 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1139,6 +1364,15 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1162,30 +1396,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>328</v>
+        <v>400</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>330</v>
+        <v>402</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>331</v>
+        <v>403</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>332</v>
+        <v>404</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>333</v>
+        <v>405</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>334</v>
+        <v>406</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>335</v>
+        <v>407</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>329</v>
+        <v>401</v>
       </c>
       <c r="B2" s="0">
         <v>71</v>

</xml_diff>

<commit_message>
corrected issue related to importing BDF events as edftype or type idiosyncratically. Now gives visual feedback related to shifted event codes in bins.
</commit_message>
<xml_diff>
--- a/SupportingDocs/AR_Parameters_for_MW_Blinks.xlsx
+++ b/SupportingDocs/AR_Parameters_for_MW_Blinks.xlsx
@@ -13,7 +13,463 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="560">
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
+  <si>
+    <t>SUBID</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>Channel(s)</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Time Window Minimum</t>
+  </si>
+  <si>
+    <t>Time Window Maximum</t>
+  </si>
+  <si>
+    <t>Window Size</t>
+  </si>
+  <si>
+    <t>Window Step</t>
+  </si>
   <si>
     <t>SUBID</t>
   </si>
@@ -1257,7 +1713,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="71">
     <border>
       <left/>
       <right/>
@@ -1316,11 +1772,30 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1373,6 +1848,25 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="68" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="69" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="70" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1396,30 +1890,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>400</v>
+        <v>552</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>402</v>
+        <v>554</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>403</v>
+        <v>555</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>404</v>
+        <v>556</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>405</v>
+        <v>557</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>406</v>
+        <v>558</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>407</v>
+        <v>559</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>401</v>
+        <v>553</v>
       </c>
       <c r="B2" s="0">
         <v>71</v>

</xml_diff>